<commit_message>
trying to figure out how to best save settings
</commit_message>
<xml_diff>
--- a/SpotifyLyricsErrors.xlsx
+++ b/SpotifyLyricsErrors.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Service</t>
   </si>
@@ -94,6 +94,30 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>http://genius.com/G-Eazy-Him-&amp;-I-lyrics</t>
+  </si>
+  <si>
+    <t>https://genius.com/G-eazy-him-and-i-lyrics</t>
+  </si>
+  <si>
+    <t>"and" instead of "&amp;"</t>
+  </si>
+  <si>
+    <t>Him &amp; I</t>
+  </si>
+  <si>
+    <t>http://genius.com/Sushi-x-Kobe-Flasker-på-flasker-lyrics</t>
+  </si>
+  <si>
+    <t>https://genius.com/Sushi-x-kobe-flasker-pa-flasker-lyrics</t>
+  </si>
+  <si>
+    <t>"a" instead of "å"</t>
+  </si>
+  <si>
+    <t>Flasker på flasker</t>
   </si>
 </sst>
 </file>
@@ -440,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +475,7 @@
     <col min="1" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -553,6 +577,46 @@
       </c>
       <c r="F5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>